<commit_message>
Db references updated and lv stations from enexis
TODO: Mobility samples from original db
</commit_message>
<xml_diff>
--- a/Data/Afrikaanderbuurt_midden_lv_stations.xlsx
+++ b/Data/Afrikaanderbuurt_midden_lv_stations.xlsx
@@ -5,23 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-buurt-scerious-game\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-buurt-serious-game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC40A363-7E34-45A7-88F3-FB21CF43C0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE04AF27-55A8-436D-8C26-E7792FCB9894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-945" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Afrikaanderbuurt_midden_lv_stat" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>currentsta</t>
   </si>
@@ -126,6 +139,12 @@
   </si>
   <si>
     <t>!elec!e_fl_station_lv!6499541792496733204</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>nominal_power</t>
   </si>
 </sst>
 </file>
@@ -159,8 +178,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,6 +196,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Results"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,340 +508,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="15"/>
+    <col min="3" max="1026" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>105130684</v>
+      </c>
+      <c r="B2">
+        <f>_xlfn.IFNA(VLOOKUP(A2,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>400</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>5.0762988130998732</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>51.54557425806523</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>14812414</v>
+      </c>
+      <c r="B3">
+        <f>_xlfn.IFNA(VLOOKUP(A3,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>315</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>5.077731394208012</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>51.54440926286491</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>14812566</v>
+      </c>
+      <c r="B4">
+        <f>_xlfn.IFNA(VLOOKUP(A4,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>5.0697513063416011</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>51.545114024493479</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>14812702</v>
+      </c>
+      <c r="B5">
+        <f>_xlfn.IFNA(VLOOKUP(A5,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>250</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>5.0742392557572638</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>51.54694016355527</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5.3981761389993001E+18</v>
+      </c>
+      <c r="B6">
+        <f>_xlfn.IFNA(VLOOKUP(A6,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>20</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>5.0773856720038726</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>51.547049010216242</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5.5853205514256896E+18</v>
+      </c>
+      <c r="B7">
+        <f>_xlfn.IFNA(VLOOKUP(A7,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>400</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>22</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>5.0704518414700042</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>51.54668157971448</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6.4995417924967301E+18</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.IFNA(VLOOKUP(A8,[1]!Table1[#All],2,FALSE),0)</f>
+        <v>630</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>20</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>22</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>5.0724700688298396</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>51.544970177047261</v>
       </c>
     </row>

</xml_diff>